<commit_message>
Arreglando subida de evento
</commit_message>
<xml_diff>
--- a/public/formulario_historico - copia.xlsx
+++ b/public/formulario_historico - copia.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="105">
   <si>
     <t>ID</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>1 - 2</t>
+  </si>
+  <si>
+    <t>5c5479fbe394015b5e3941e7</t>
   </si>
 </sst>
 </file>
@@ -720,7 +723,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1445,6 +1448,71 @@
         <v>28</v>
       </c>
     </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>33</v>
+      </c>
+      <c r="R12" t="s">
+        <v>34</v>
+      </c>
+      <c r="S12" t="s">
+        <v>28</v>
+      </c>
+      <c r="T12" t="s">
+        <v>28</v>
+      </c>
+      <c r="U12" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>

</xml_diff>